<commit_message>
Updated the RTM document according to the CYRS Signed-off-by: Moustafa Ghareeb <moustafa.ghareeb.hpg@gmail.com>
</commit_message>
<xml_diff>
--- a/Software Specification/RTM.xlsx
+++ b/Software Specification/RTM.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Digital_Elevator\Software Specification\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28D9AC82-817B-45CF-911A-5E365FBD89D4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5954C44-7F31-4031-A6EB-B4594162B88B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{6C68D336-FBF6-4C75-84CC-7B5C006C0E24}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="18">
   <si>
     <t>Digital Elevator_RTM</t>
   </si>
@@ -63,19 +63,28 @@
     <t xml:space="preserve">The user has 3 trials then blocked for 5 sec </t>
   </si>
   <si>
-    <t xml:space="preserve">Calling the ELEV is done by Up/Down switches </t>
-  </si>
-  <si>
     <t xml:space="preserve"> A reset for the whole system is done when pressing On/Of button for 2 sec </t>
   </si>
   <si>
-    <t>When pass for the given ID is correct the system should give display OK and start moving up / Down as the request from the user.</t>
-  </si>
-  <si>
     <t>When the user calling the elevator for the first time , the system will acquire him to enter New ID “First name ” by max 10 character and a new password “****” 4 digits then he is OK to use the Elevator</t>
   </si>
   <si>
     <t>When user is setting the ID is it already taken system has to ask for another one.</t>
+  </si>
+  <si>
+    <t>Req _ DIGELV _CYRS_01_V1.0</t>
+  </si>
+  <si>
+    <t>Req _ DIGELV _CYRS_02_V1.0</t>
+  </si>
+  <si>
+    <t>Req _ DIGELV _CYRS_03_V1.0</t>
+  </si>
+  <si>
+    <t>Req _ DIGELV _CYRS_04_V1.0</t>
+  </si>
+  <si>
+    <t>When pass for the given ID is correct the system should give display OK and start moving up / Down as the request from the user. Calling the ELEV is done by Up/Down switches.</t>
   </si>
 </sst>
 </file>
@@ -162,7 +171,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -170,12 +179,6 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -186,13 +189,22 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -508,17 +520,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A441A6F4-93EC-4962-B844-0F7E31CE1CB0}">
-  <dimension ref="A1:G16"/>
+  <dimension ref="A1:G15"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+      <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="3.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="91.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="9.140625" style="1"/>
+    <col min="3" max="3" width="13.85546875" style="1" customWidth="1"/>
+    <col min="4" max="4" width="18.28515625" style="1" customWidth="1"/>
     <col min="5" max="5" width="11.7109375" style="1" customWidth="1"/>
     <col min="6" max="16384" width="9.140625" style="1"/>
   </cols>
@@ -544,155 +557,158 @@
       <c r="B3" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C3" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="3"/>
-      <c r="E3" s="3" t="s">
+      <c r="D3" s="8"/>
+      <c r="E3" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="F3" s="3"/>
+      <c r="F3" s="8"/>
     </row>
     <row r="4" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="8">
+      <c r="A4" s="6">
         <v>1</v>
       </c>
-      <c r="B4" s="10" t="s">
+      <c r="B4" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="4"/>
-      <c r="D4" s="4"/>
-      <c r="E4" s="4"/>
-      <c r="F4" s="4"/>
+      <c r="C4" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="D4" s="10"/>
+      <c r="E4" s="6"/>
+      <c r="F4" s="6"/>
     </row>
     <row r="5" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A5" s="8">
+      <c r="A5" s="6">
         <v>2</v>
       </c>
-      <c r="B5" s="10" t="s">
+      <c r="B5" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="4"/>
-      <c r="D5" s="4"/>
-      <c r="E5" s="4"/>
-      <c r="F5" s="4"/>
+      <c r="C5" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="D5" s="11"/>
+      <c r="E5" s="6"/>
+      <c r="F5" s="6"/>
     </row>
     <row r="6" spans="1:7" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A6" s="8">
+      <c r="A6" s="6">
         <v>3</v>
       </c>
-      <c r="B6" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="C6" s="4"/>
-      <c r="D6" s="4"/>
-      <c r="E6" s="4"/>
-      <c r="F6" s="4"/>
+      <c r="B6" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6" s="11"/>
+      <c r="D6" s="11"/>
+      <c r="E6" s="6"/>
+      <c r="F6" s="6"/>
     </row>
     <row r="7" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A7" s="8">
+      <c r="A7" s="6">
         <v>4</v>
       </c>
-      <c r="B7" s="10" t="s">
+      <c r="B7" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="C7" s="4"/>
-      <c r="D7" s="4"/>
-      <c r="E7" s="4"/>
-      <c r="F7" s="4"/>
+      <c r="C7" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="D7" s="11"/>
+      <c r="E7" s="6"/>
+      <c r="F7" s="6"/>
     </row>
     <row r="8" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A8" s="8">
+      <c r="A8" s="6">
         <v>5</v>
       </c>
-      <c r="B8" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="C8" s="4"/>
-      <c r="D8" s="4"/>
-      <c r="E8" s="4"/>
-      <c r="F8" s="4"/>
+      <c r="B8" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="C8" s="11"/>
+      <c r="D8" s="11"/>
+      <c r="E8" s="6"/>
+      <c r="F8" s="6"/>
     </row>
     <row r="9" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A9" s="8">
+      <c r="A9" s="6">
         <v>6</v>
       </c>
-      <c r="B9" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="C9" s="4"/>
-      <c r="D9" s="4"/>
-      <c r="E9" s="4"/>
-      <c r="F9" s="4"/>
+      <c r="B9" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="C9" s="11"/>
+      <c r="D9" s="11"/>
+      <c r="E9" s="6"/>
+      <c r="F9" s="6"/>
     </row>
     <row r="10" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A10" s="8">
+      <c r="A10" s="6">
         <v>7</v>
       </c>
-      <c r="B10" s="8" t="s">
+      <c r="B10" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="C10" s="4"/>
-      <c r="D10" s="4"/>
-      <c r="E10" s="4"/>
-      <c r="F10" s="4"/>
+      <c r="C10" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="D10" s="11"/>
+      <c r="E10" s="6"/>
+      <c r="F10" s="6"/>
     </row>
     <row r="11" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A11" s="8">
+      <c r="A11" s="6">
         <v>8</v>
       </c>
-      <c r="B11" s="8" t="s">
+      <c r="B11" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="C11" s="4"/>
-      <c r="D11" s="4"/>
-      <c r="E11" s="4"/>
-      <c r="F11" s="4"/>
+      <c r="C11" s="11"/>
+      <c r="D11" s="11"/>
+      <c r="E11" s="6"/>
+      <c r="F11" s="6"/>
     </row>
     <row r="12" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A12" s="8">
+      <c r="A12" s="6">
         <v>9</v>
       </c>
-      <c r="B12" s="8" t="s">
+      <c r="B12" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="C12" s="4"/>
-      <c r="D12" s="4"/>
-      <c r="E12" s="4"/>
-      <c r="F12" s="4"/>
-    </row>
-    <row r="13" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A13" s="8">
-        <v>10</v>
-      </c>
-      <c r="B13" s="8" t="s">
-        <v>11</v>
-      </c>
+      <c r="C12" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="D12" s="11"/>
+      <c r="E12" s="6"/>
+      <c r="F12" s="6"/>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" s="4"/>
+      <c r="B13" s="5"/>
       <c r="C13" s="4"/>
       <c r="D13" s="4"/>
       <c r="E13" s="4"/>
       <c r="F13" s="4"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" s="6"/>
-      <c r="B14" s="7"/>
-      <c r="C14" s="6"/>
-      <c r="D14" s="6"/>
-      <c r="E14" s="6"/>
-      <c r="F14" s="6"/>
-      <c r="G14" s="6"/>
+      <c r="B14" s="3"/>
+      <c r="G14" s="4"/>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B15" s="5"/>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B16" s="5"/>
+      <c r="B15" s="3"/>
     </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="8">
+    <mergeCell ref="C7:D9"/>
+    <mergeCell ref="C10:D11"/>
+    <mergeCell ref="C12:D12"/>
     <mergeCell ref="C3:D3"/>
     <mergeCell ref="E3:F3"/>
     <mergeCell ref="B1:E2"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="C5:D6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Updating the RTM according to the SRS Signed-off-by: Moustafa Ghareeb <moustafa.ghareeb.hpg@gmail.com>
</commit_message>
<xml_diff>
--- a/Software Specification/RTM.xlsx
+++ b/Software Specification/RTM.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Digital_Elevator\Software Specification\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5954C44-7F31-4031-A6EB-B4594162B88B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C813159D-896D-456B-9384-3D02C62BA07F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{6C68D336-FBF6-4C75-84CC-7B5C006C0E24}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="23">
   <si>
     <t>Digital Elevator_RTM</t>
   </si>
@@ -85,6 +85,24 @@
   </si>
   <si>
     <t>When pass for the given ID is correct the system should give display OK and start moving up / Down as the request from the user. Calling the ELEV is done by Up/Down switches.</t>
+  </si>
+  <si>
+    <t>[DIGELV_SRS_001_V1.0]</t>
+  </si>
+  <si>
+    <t>[DIGELV_SRS_008_V1.0]</t>
+  </si>
+  <si>
+    <t>[DIGELV_SRS_009_V1.0]</t>
+  </si>
+  <si>
+    <t>[DIGELV_SRS_002_V1.0][DIGELV_SRS_003_V1.0]
+[DIGELV_SRS_004_V1.0]
+[DIGELV_SRS_005_V1.0]</t>
+  </si>
+  <si>
+    <t>[DIGELV_SRS_006_V1.0]
+[DIGELV_SRS_007_V1.0]</t>
   </si>
 </sst>
 </file>
@@ -171,7 +189,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -194,6 +212,9 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -204,7 +225,10 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -523,7 +547,7 @@
   <dimension ref="A1:G15"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="I6" sqref="I6"/>
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -532,23 +556,24 @@
     <col min="2" max="2" width="91.28515625" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="13.85546875" style="1" customWidth="1"/>
     <col min="4" max="4" width="18.28515625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="11.7109375" style="1" customWidth="1"/>
-    <col min="6" max="16384" width="9.140625" style="1"/>
+    <col min="5" max="5" width="24.85546875" style="1" customWidth="1"/>
+    <col min="6" max="6" width="0.28515625" style="1" customWidth="1"/>
+    <col min="7" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="9" t="s">
+      <c r="B1" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="9"/>
-      <c r="D1" s="9"/>
-      <c r="E1" s="9"/>
+      <c r="C1" s="10"/>
+      <c r="D1" s="10"/>
+      <c r="E1" s="10"/>
     </row>
     <row r="2" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="9"/>
-      <c r="C2" s="9"/>
-      <c r="D2" s="9"/>
-      <c r="E2" s="9"/>
+      <c r="B2" s="10"/>
+      <c r="C2" s="10"/>
+      <c r="D2" s="10"/>
+      <c r="E2" s="10"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
@@ -557,14 +582,14 @@
       <c r="B3" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="8" t="s">
+      <c r="C3" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="8"/>
-      <c r="E3" s="8" t="s">
+      <c r="D3" s="9"/>
+      <c r="E3" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="F3" s="8"/>
+      <c r="F3" s="9"/>
     </row>
     <row r="4" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="6">
@@ -573,12 +598,14 @@
       <c r="B4" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="10" t="s">
+      <c r="C4" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="D4" s="10"/>
-      <c r="E4" s="6"/>
-      <c r="F4" s="6"/>
+      <c r="D4" s="11"/>
+      <c r="E4" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="F4" s="12"/>
     </row>
     <row r="5" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" s="6">
@@ -587,24 +614,26 @@
       <c r="B5" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="11" t="s">
+      <c r="C5" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="D5" s="11"/>
-      <c r="E5" s="6"/>
-      <c r="F5" s="6"/>
-    </row>
-    <row r="6" spans="1:7" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="D5" s="8"/>
+      <c r="E5" s="12"/>
+      <c r="F5" s="12"/>
+    </row>
+    <row r="6" spans="1:7" ht="78.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="6">
         <v>3</v>
       </c>
       <c r="B6" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="C6" s="11"/>
-      <c r="D6" s="11"/>
-      <c r="E6" s="6"/>
-      <c r="F6" s="6"/>
+      <c r="C6" s="8"/>
+      <c r="D6" s="8"/>
+      <c r="E6" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="F6" s="13"/>
     </row>
     <row r="7" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A7" s="6">
@@ -613,12 +642,14 @@
       <c r="B7" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="C7" s="11" t="s">
+      <c r="C7" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="D7" s="11"/>
-      <c r="E7" s="6"/>
-      <c r="F7" s="6"/>
+      <c r="D7" s="8"/>
+      <c r="E7" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="F7" s="12"/>
     </row>
     <row r="8" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A8" s="6">
@@ -627,10 +658,10 @@
       <c r="B8" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="C8" s="11"/>
-      <c r="D8" s="11"/>
-      <c r="E8" s="6"/>
-      <c r="F8" s="6"/>
+      <c r="C8" s="8"/>
+      <c r="D8" s="8"/>
+      <c r="E8" s="8"/>
+      <c r="F8" s="12"/>
     </row>
     <row r="9" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A9" s="6">
@@ -639,10 +670,10 @@
       <c r="B9" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="C9" s="11"/>
-      <c r="D9" s="11"/>
-      <c r="E9" s="6"/>
-      <c r="F9" s="6"/>
+      <c r="C9" s="8"/>
+      <c r="D9" s="8"/>
+      <c r="E9" s="8"/>
+      <c r="F9" s="12"/>
     </row>
     <row r="10" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A10" s="6">
@@ -651,12 +682,14 @@
       <c r="B10" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="C10" s="11" t="s">
+      <c r="C10" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="D10" s="11"/>
-      <c r="E10" s="6"/>
-      <c r="F10" s="6"/>
+      <c r="D10" s="8"/>
+      <c r="E10" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="F10" s="8"/>
     </row>
     <row r="11" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A11" s="6">
@@ -665,10 +698,10 @@
       <c r="B11" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="C11" s="11"/>
-      <c r="D11" s="11"/>
-      <c r="E11" s="6"/>
-      <c r="F11" s="6"/>
+      <c r="C11" s="8"/>
+      <c r="D11" s="8"/>
+      <c r="E11" s="8"/>
+      <c r="F11" s="8"/>
     </row>
     <row r="12" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A12" s="6">
@@ -677,12 +710,14 @@
       <c r="B12" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="C12" s="11" t="s">
+      <c r="C12" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="D12" s="11"/>
-      <c r="E12" s="6"/>
-      <c r="F12" s="6"/>
+      <c r="D12" s="8"/>
+      <c r="E12" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="F12" s="8"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="4"/>
@@ -700,15 +735,19 @@
       <c r="B15" s="3"/>
     </row>
   </sheetData>
-  <mergeCells count="8">
+  <mergeCells count="12">
+    <mergeCell ref="B1:E2"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="C5:D6"/>
+    <mergeCell ref="E6:F6"/>
     <mergeCell ref="C7:D9"/>
     <mergeCell ref="C10:D11"/>
     <mergeCell ref="C12:D12"/>
     <mergeCell ref="C3:D3"/>
     <mergeCell ref="E3:F3"/>
-    <mergeCell ref="B1:E2"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="C5:D6"/>
+    <mergeCell ref="E12:F12"/>
+    <mergeCell ref="E7:E9"/>
+    <mergeCell ref="E10:F11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Updating the RTM according to the new SRS modifications Signed-off-by: Moustafa Ghareeb <moustafa.ghareeb.hpg@gmail.com>
</commit_message>
<xml_diff>
--- a/Software Specification/RTM.xlsx
+++ b/Software Specification/RTM.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Digital_Elevator\Software Specification\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED440CA9-0823-40D9-A334-7A36E2D1301C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C359307-3304-4EC8-A94A-5ACCEEC41818}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{6C68D336-FBF6-4C75-84CC-7B5C006C0E24}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
   <si>
     <t>Digital Elevator_RTM</t>
   </si>
@@ -72,37 +72,48 @@
     <t>When user is setting the ID is it already taken system has to ask for another one.</t>
   </si>
   <si>
-    <t>Req _ DIGELV _CYRS_01_V1.0</t>
-  </si>
-  <si>
-    <t>Req _ DIGELV _CYRS_02_V1.0</t>
-  </si>
-  <si>
-    <t>Req _ DIGELV _CYRS_03_V1.0</t>
-  </si>
-  <si>
-    <t>Req _ DIGELV _CYRS_04_V1.0</t>
-  </si>
-  <si>
     <t>When pass for the given ID is correct the system should give display OK and start moving up / Down as the request from the user. Calling the ELEV is done by Up/Down switches.</t>
   </si>
   <si>
-    <t>[DIGELV_SRS_001_V1.0]</t>
-  </si>
-  <si>
-    <t>[DIGELV_SRS_008_V1.0]</t>
-  </si>
-  <si>
-    <t>[DIGELV_SRS_009_V1.0]</t>
-  </si>
-  <si>
-    <t>[DIGELV_SRS_002_V1.0][DIGELV_SRS_003_V1.0]
+    <t xml:space="preserve"> DIGELV _CYRS_01_V1.0</t>
+  </si>
+  <si>
+    <t>DIGELV _CYRS_02_V1.0</t>
+  </si>
+  <si>
+    <t>DIGELV _CYRS_03_V1.0</t>
+  </si>
+  <si>
+    <t>DIGELV _CYRS_04_V1.0</t>
+  </si>
+  <si>
+    <t>DIGELV _CYRS_05_V1.0</t>
+  </si>
+  <si>
+    <t>[DIGELV_SRS_001_V1.0]
+[DIGELV_SRS_002_V1.0]</t>
+  </si>
+  <si>
+    <t>[DIGELV_SRS_003_V1.0]
 [DIGELV_SRS_004_V1.0]
-[DIGELV_SRS_005_V1.0]</t>
-  </si>
-  <si>
-    <t>[DIGELV_SRS_006_V1.0]
-[DIGELV_SRS_007_V1.0]</t>
+[DIGELV_SRS_005_V1.0]
+[DIGELV_SRS_006_V1.0]
+[DIGELV_SRS_007_V1.0]
+[DIGELV_SRS_007_V1.0]
+[DIGELV_SRS_009_V1.0]
+[DIGELV_SRS_010_V1.0]
+[DIGELV_SRS_011_V1.0]</t>
+  </si>
+  <si>
+    <t>[DIGELV_SRS_012_V1.0]
+[DIGELV_SRS_013_V1.0]</t>
+  </si>
+  <si>
+    <t>[DIGELV_SRS_014_V1.0]
+[DIGELV_SRS_015_V1.0]</t>
+  </si>
+  <si>
+    <t>[DIGELV_SRS_016_V1.0]</t>
   </si>
 </sst>
 </file>
@@ -215,20 +226,20 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -605,7 +616,7 @@
   <dimension ref="A1:G15"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -620,18 +631,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="9" t="s">
+      <c r="B1" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="9"/>
-      <c r="D1" s="9"/>
-      <c r="E1" s="9"/>
+      <c r="C1" s="12"/>
+      <c r="D1" s="12"/>
+      <c r="E1" s="12"/>
     </row>
     <row r="2" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="9"/>
-      <c r="C2" s="9"/>
-      <c r="D2" s="9"/>
-      <c r="E2" s="9"/>
+      <c r="B2" s="12"/>
+      <c r="C2" s="12"/>
+      <c r="D2" s="12"/>
+      <c r="E2" s="12"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
@@ -640,14 +651,14 @@
       <c r="B3" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="13" t="s">
+      <c r="C3" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="13"/>
-      <c r="E3" s="13" t="s">
+      <c r="D3" s="10"/>
+      <c r="E3" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="F3" s="13"/>
+      <c r="F3" s="10"/>
     </row>
     <row r="4" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="6">
@@ -656,12 +667,12 @@
       <c r="B4" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="D4" s="10"/>
-      <c r="E4" s="8" t="s">
-        <v>18</v>
+      <c r="C4" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4" s="13"/>
+      <c r="E4" s="11" t="s">
+        <v>19</v>
       </c>
       <c r="F4" s="8"/>
     </row>
@@ -672,26 +683,26 @@
       <c r="B5" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="11" t="s">
-        <v>14</v>
-      </c>
-      <c r="D5" s="11"/>
-      <c r="E5" s="8"/>
+      <c r="C5" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="D5" s="9"/>
+      <c r="E5" s="9"/>
       <c r="F5" s="8"/>
     </row>
-    <row r="6" spans="1:7" ht="78.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" ht="159" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="6">
         <v>3</v>
       </c>
       <c r="B6" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="C6" s="11"/>
-      <c r="D6" s="11"/>
-      <c r="E6" s="12" t="s">
-        <v>21</v>
-      </c>
-      <c r="F6" s="12"/>
+      <c r="C6" s="9"/>
+      <c r="D6" s="9"/>
+      <c r="E6" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="F6" s="11"/>
     </row>
     <row r="7" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A7" s="6">
@@ -700,12 +711,12 @@
       <c r="B7" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="C7" s="11" t="s">
-        <v>15</v>
-      </c>
-      <c r="D7" s="11"/>
-      <c r="E7" s="12" t="s">
-        <v>22</v>
+      <c r="C7" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="D7" s="9"/>
+      <c r="E7" s="11" t="s">
+        <v>21</v>
       </c>
       <c r="F7" s="8"/>
     </row>
@@ -716,9 +727,9 @@
       <c r="B8" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="C8" s="11"/>
-      <c r="D8" s="11"/>
-      <c r="E8" s="11"/>
+      <c r="C8" s="9"/>
+      <c r="D8" s="9"/>
+      <c r="E8" s="9"/>
       <c r="F8" s="8"/>
     </row>
     <row r="9" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
@@ -726,11 +737,11 @@
         <v>6</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="C9" s="11"/>
-      <c r="D9" s="11"/>
-      <c r="E9" s="11"/>
+        <v>13</v>
+      </c>
+      <c r="C9" s="9"/>
+      <c r="D9" s="9"/>
+      <c r="E9" s="9"/>
       <c r="F9" s="8"/>
     </row>
     <row r="10" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
@@ -740,14 +751,14 @@
       <c r="B10" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="C10" s="11" t="s">
-        <v>16</v>
-      </c>
-      <c r="D10" s="11"/>
+      <c r="C10" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="D10" s="9"/>
       <c r="E10" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="F10" s="11"/>
+        <v>22</v>
+      </c>
+      <c r="F10" s="9"/>
     </row>
     <row r="11" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A11" s="6">
@@ -756,10 +767,10 @@
       <c r="B11" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="C11" s="11"/>
-      <c r="D11" s="11"/>
-      <c r="E11" s="11"/>
-      <c r="F11" s="11"/>
+      <c r="C11" s="9"/>
+      <c r="D11" s="9"/>
+      <c r="E11" s="9"/>
+      <c r="F11" s="9"/>
     </row>
     <row r="12" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A12" s="6">
@@ -768,14 +779,14 @@
       <c r="B12" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="C12" s="11" t="s">
-        <v>16</v>
-      </c>
-      <c r="D12" s="11"/>
-      <c r="E12" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="F12" s="11"/>
+      <c r="C12" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="D12" s="9"/>
+      <c r="E12" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="F12" s="9"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="4"/>
@@ -793,7 +804,13 @@
       <c r="B15" s="3"/>
     </row>
   </sheetData>
-  <mergeCells count="12">
+  <mergeCells count="13">
+    <mergeCell ref="B1:E2"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="C5:D6"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="C7:D9"/>
+    <mergeCell ref="E4:E5"/>
     <mergeCell ref="C10:D11"/>
     <mergeCell ref="C12:D12"/>
     <mergeCell ref="C3:D3"/>
@@ -801,11 +818,6 @@
     <mergeCell ref="E12:F12"/>
     <mergeCell ref="E7:E9"/>
     <mergeCell ref="E10:F11"/>
-    <mergeCell ref="B1:E2"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="C5:D6"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="C7:D9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>